<commit_message>
Iterated on music, fish colors, more vo stuff.
</commit_message>
<xml_diff>
--- a/floppy_fish_godot/UI/floppy_fish_localization.xlsx
+++ b/floppy_fish_godot/UI/floppy_fish_localization.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -32,6 +32,36 @@
   </si>
   <si>
     <t xml:space="preserve">Oh, buoy!  You did it!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start_controls1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sometimes games with the simplest control schemes are the most difficult.  For example, in Getting Over It with Bennett Foddy, the only thing you do is move the mouse, but the complex interactions with physics allow for very in-depth movement mechanics. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">start_controls2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this game, designed to capture the Foddian spirit, you simply have 2 controls: flop left and flop right.  You can use arrow keys, A and D, or the mouse buttons to flip and flop.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start_controls3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are, quite literally, a fish out of water.  I was planning to have the the movement driven entirely by the physics of the fish contacting the world, but, believe it or not, that was more uncontrollable than what you’re playing now.  You’d flip and flop upward with no practical way to progress forward.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start_controls4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then I realized that, while not as effective as in water, a tail flapping back and forth would create some sort of forward momentum due to the air being pushed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start_controls5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I’m not sure how physically accurate this is, but it does seem slightly more plausible than a man lifting his entire body weight and that of a cauldron up using just a hammer.</t>
   </si>
 </sst>
 </file>
@@ -127,14 +157,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="86.84"/>
   </cols>
   <sheetData>
@@ -152,6 +183,46 @@
       </c>
       <c r="B2" s="0" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added red herring joke (bucket, splash sounds, narration, material), fixed vo line about tail in water, added more bins.
</commit_message>
<xml_diff>
--- a/floppy_fish_godot/UI/floppy_fish_localization.xlsx
+++ b/floppy_fish_godot/UI/floppy_fish_localization.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t xml:space="preserve">Keep floundering!  You’re bound to make it somewhere eventually.  Maybe not where you wanted to go, but somewhere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red_herring1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you’re at all familiar with logical fallacies, you’d realize what we’re looking at here is clearly a red herring – something to divert attention away from the real issue at hand.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red_herring2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the real issue at hand?  I’m not sure.  I’m too distracted by the red fish flopping around.</t>
   </si>
 </sst>
 </file>
@@ -112,6 +124,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -263,16 +276,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="86.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="86.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,6 +390,22 @@
       </c>
       <c r="B13" s="0" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added VO about losing progress.  Added analog mouse support.  Replaced a bunch of boxes with lobster traps and stuff.  Left and right bumpers flop left and right.  Left and right triggers and left stick can also be used to flop.  Improved volume sliders and checkboxes.
</commit_message>
<xml_diff>
--- a/floppy_fish_godot/UI/floppy_fish_localization.xlsx
+++ b/floppy_fish_godot/UI/floppy_fish_localization.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t xml:space="preserve">What is the real issue at hand?  I’m not sure.  I’m too distracted by the red fish flopping around.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lost_progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A key element of Foddian games is the ability to fall down and lose progress.  Designing levels around fish flopping proved difficult to create that kind of verticality, but, as you’ve just demonstrated, it is still quite easy to lose progress on a horizontal surface.</t>
   </si>
 </sst>
 </file>
@@ -276,10 +282,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -408,6 +414,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>